<commit_message>
update to data dictionary - high level sample included
</commit_message>
<xml_diff>
--- a/dummy_data_f2_datadict.xlsx
+++ b/dummy_data_f2_datadict.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="151">
   <si>
     <t>Description</t>
   </si>
@@ -112,9 +112,6 @@
     <t>SF of building area</t>
   </si>
   <si>
-    <t>1 if te project have a sf component</t>
-  </si>
-  <si>
     <t>Year of the project start date</t>
   </si>
   <si>
@@ -371,13 +368,117 @@
   </si>
   <si>
     <t>This is the unique identifier for each data point</t>
+  </si>
+  <si>
+    <t>Valley Fair - Predev</t>
+  </si>
+  <si>
+    <t>JVE</t>
+  </si>
+  <si>
+    <t>NW</t>
+  </si>
+  <si>
+    <t>Flagship</t>
+  </si>
+  <si>
+    <t>Additional Criteria Needed</t>
+  </si>
+  <si>
+    <t>Board Date</t>
+  </si>
+  <si>
+    <t>Construction Start Date</t>
+  </si>
+  <si>
+    <t>Construction End Date</t>
+  </si>
+  <si>
+    <t>Tenant Info (if applicable)</t>
+  </si>
+  <si>
+    <t>New Tenant (number)</t>
+  </si>
+  <si>
+    <t>New Tenant (SF)</t>
+  </si>
+  <si>
+    <t>New Tenant (rent - MR)</t>
+  </si>
+  <si>
+    <t>New Tenant (rent - CAM)</t>
+  </si>
+  <si>
+    <t>New Tenant (rent - MKT)</t>
+  </si>
+  <si>
+    <t>New Tenant (rent - TAX)</t>
+  </si>
+  <si>
+    <t>=[TM1 PULL]OR[User Input]</t>
+  </si>
+  <si>
+    <t>If we can mark development tenants in system we can use TM1; otherwise manually enter</t>
+  </si>
+  <si>
+    <t>Westfield Ownership (%)</t>
+  </si>
+  <si>
+    <t>=[TM1 PULL]</t>
+  </si>
+  <si>
+    <t>SAMPLE</t>
+  </si>
+  <si>
+    <t>General Rates</t>
+  </si>
+  <si>
+    <t>Capitalized Interest Rate</t>
+  </si>
+  <si>
+    <t>Corporate Overhead Rate</t>
+  </si>
+  <si>
+    <t>Leasing Cost Rates</t>
+  </si>
+  <si>
+    <t>Partnership Calc Rates</t>
+  </si>
+  <si>
+    <t>These rates differ depending on partner</t>
+  </si>
+  <si>
+    <t>There are other rates that differ depending on partner and this model should pick that up when the partner is tagged</t>
+  </si>
+  <si>
+    <t>Partner</t>
+  </si>
+  <si>
+    <t>Will be pulled from system when BU is specified</t>
+  </si>
+  <si>
+    <t>Discount Rate</t>
+  </si>
+  <si>
+    <t>May differ depending on BU, may have master rate, or may have option to enter manually</t>
+  </si>
+  <si>
+    <t>Terminal Rate</t>
+  </si>
+  <si>
+    <t>1 if the project have a sf component</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="169" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -513,6 +614,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u val="singleAccounting"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -695,7 +812,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -810,8 +927,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -854,15 +995,44 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="11"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="8" xfId="15" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="18" fillId="8" borderId="8" xfId="15" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="10" xfId="15" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="167" fontId="16" fillId="0" borderId="11" xfId="42" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -890,6 +1060,7 @@
     <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Comma" xfId="42" builtinId="3"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
@@ -1203,10 +1374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:I80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1215,9 +1386,10 @@
     <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="112.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="69" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="17.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1230,8 +1402,11 @@
       <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I1" s="14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
@@ -1242,10 +1417,13 @@
         <v>28</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="I2">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1256,8 +1434,11 @@
         <v>28</v>
       </c>
       <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>20</v>
       </c>
@@ -1268,102 +1449,126 @@
         <v>28</v>
       </c>
       <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I4" s="20">
+        <v>900000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>32</v>
+        <v>150</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>12297</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I12" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>2</v>
@@ -1371,79 +1576,92 @@
       <c r="D13" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H13" s="10">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="I13" s="8">
+        <f ca="1">SUM(I12,I14:I51)*(H13/12)*24</f>
+        <v>66.879440055999993</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>3.33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I18" s="5">
+        <v>511.83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>10</v>
@@ -1451,101 +1669,130 @@
       <c r="D20" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H20" s="6">
+        <v>0.08</v>
+      </c>
+      <c r="I20" s="8">
+        <f ca="1">$I$18*H20</f>
+        <v>40.946399999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H21" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="I21" s="8">
+        <f ca="1">$I$18*H21</f>
+        <v>10.236599999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I22" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I23" s="8"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H24" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="I24" s="8">
+        <f ca="1">SUM(I12,I14:I23,I25:I51)*H24</f>
+        <v>22.135736999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I25" s="8"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I26" s="8"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I27" s="8"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I28" s="8"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>12</v>
@@ -1553,57 +1800,62 @@
       <c r="D29" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I29" s="8"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I30" s="8"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I31" s="8"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B32" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I32" s="8"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I33" s="8"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>4</v>
@@ -1611,192 +1863,409 @@
       <c r="D34" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I34" s="9">
+        <v>6.66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I35" s="9">
+        <v>16.239999999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I36" s="9">
+        <v>4.04</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B37" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I37" s="8"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B38" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I38" s="8"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B39" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H39" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="I39" s="8">
+        <f ca="1">$I$18*H39</f>
+        <v>15.354899999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B40" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B41" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I41" s="7">
+        <v>24.41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B43" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B44" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B46" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I46" s="7">
+        <v>4.66</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B47" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I47" s="7">
+        <v>95.58</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B48" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I48" s="7">
+        <v>4.57</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B49" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B50" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B51" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="I51" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I52" s="19">
+        <f ca="1">SUM(I12:I51)</f>
+        <v>826.87307705599994</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="I53" s="18"/>
+    </row>
+    <row r="58" spans="1:9" ht="17.25" x14ac:dyDescent="0.4">
+      <c r="B58" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C58" s="15"/>
+      <c r="D58" s="15"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B59" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B60" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B61" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B62" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B63" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D63" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B64" s="11"/>
+      <c r="C64" s="2"/>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D67" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B69" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B72" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="12" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B77" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D77" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B78" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D78" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B79" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D79" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B80" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D80" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>